<commit_message>
Agregados triggers de inserción
Agregados todos los triggers de inserción, cambiados los create tables para que todos tengan el schema correcto. Faltan los triggers de update. Actualizada la lista de pendientes
</commit_message>
<xml_diff>
--- a/LISTA DE PENDIENTES.xlsx
+++ b/LISTA DE PENDIENTES.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43E57F05-F872-419E-A96D-6C6CA93246FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TABLAS" sheetId="6" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
   <si>
     <t>ID</t>
   </si>
@@ -348,13 +347,19 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Alvaro</t>
+  </si>
+  <si>
+    <t>faltan los de update, inserts ya hechos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +413,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -610,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -656,58 +669,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -736,22 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -760,9 +710,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1042,7 +1056,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6C1628-72ED-4D56-9DEB-53E6C60D570F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1051,14 +1065,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="30" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" style="46" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" style="30" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="46" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" style="46" customWidth="1"/>
-    <col min="7" max="7" width="3.85546875" style="46" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" style="30" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="30" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="30" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="30" customWidth="1"/>
     <col min="9" max="9" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" customWidth="1"/>
     <col min="11" max="11" width="48.140625" bestFit="1" customWidth="1"/>
@@ -1066,71 +1080,71 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="43"/>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
       <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="58" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="61" t="s">
+      <c r="G3" s="47"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="40" t="s">
         <v>77</v>
       </c>
       <c r="J3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="43">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="41" t="s">
         <v>107</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="43">
+      <c r="E4" s="27">
         <v>14</v>
       </c>
-      <c r="F4" s="48" t="s">
+      <c r="F4" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="32" t="s">
         <v>98</v>
       </c>
       <c r="I4" s="9" t="s">
@@ -1140,26 +1154,26 @@
       <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+      <c r="A5" s="28">
         <v>2</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="28" t="s">
         <v>107</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="28">
         <v>15</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33" t="s">
         <v>99</v>
       </c>
       <c r="I5" s="9" t="s">
@@ -1168,26 +1182,26 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
+      <c r="A6" s="27">
         <v>3</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="27">
         <v>16</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48" t="s">
+      <c r="G6" s="32"/>
+      <c r="H6" s="32" t="s">
         <v>100</v>
       </c>
       <c r="I6" s="9" t="s">
@@ -1196,26 +1210,26 @@
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
+      <c r="A7" s="28">
         <v>4</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C7" s="44" t="s">
+      <c r="C7" s="28" t="s">
         <v>107</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="28">
         <v>17</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49" t="s">
+      <c r="G7" s="33"/>
+      <c r="H7" s="33" t="s">
         <v>101</v>
       </c>
       <c r="I7" s="9" t="s">
@@ -1224,26 +1238,26 @@
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43">
+      <c r="A8" s="27">
         <v>5</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="28" t="s">
         <v>107</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="27">
         <v>18</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49" t="s">
+      <c r="G8" s="33"/>
+      <c r="H8" s="33" t="s">
         <v>102</v>
       </c>
       <c r="I8" s="9" t="s">
@@ -1252,26 +1266,26 @@
       <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
+      <c r="A9" s="28">
         <v>6</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="28">
         <v>19</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48" t="s">
+      <c r="G9" s="32"/>
+      <c r="H9" s="32" t="s">
         <v>103</v>
       </c>
       <c r="I9" s="11" t="s">
@@ -1280,26 +1294,26 @@
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="43">
+      <c r="A10" s="27">
         <v>7</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="43">
+      <c r="E10" s="27">
         <v>20</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48" t="s">
+      <c r="G10" s="32"/>
+      <c r="H10" s="32" t="s">
         <v>104</v>
       </c>
       <c r="I10" s="9" t="s">
@@ -1308,26 +1322,26 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
+      <c r="A11" s="28">
         <v>8</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E11" s="44">
+      <c r="E11" s="28">
         <v>21</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48" t="s">
+      <c r="G11" s="32"/>
+      <c r="H11" s="32" t="s">
         <v>105</v>
       </c>
       <c r="I11" s="9" t="s">
@@ -1336,172 +1350,172 @@
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="43">
+      <c r="A12" s="27">
         <v>9</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="9"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
+      <c r="A13" s="28">
         <v>10</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="9"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="43">
+      <c r="A14" s="27">
         <v>11</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="28" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
       <c r="I14" s="9"/>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
+      <c r="A15" s="28">
         <v>12</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="27" t="s">
         <v>107</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="43"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="9"/>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="43">
+      <c r="A16" s="27">
         <v>13</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C16" s="44" t="s">
+      <c r="C16" s="28" t="s">
         <v>107</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="9"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="C17" s="43"/>
+      <c r="A17" s="28"/>
+      <c r="C17" s="27"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
       <c r="I17" s="9"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="27"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
       <c r="I18" s="9"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="28"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="27"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="49"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
       <c r="I19" s="9"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="28"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="11"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="49"/>
-      <c r="H20" s="49"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
       <c r="I20" s="9"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="28"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="11"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
       <c r="I21" s="9"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="45"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="45"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="10"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
       <c r="I22" s="10"/>
       <c r="J22" s="3"/>
     </row>
@@ -1520,33 +1534,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" customWidth="1"/>
     <col min="5" max="5" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
       <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
       <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1565,10 +1580,10 @@
       <c r="A4" s="20">
         <v>1</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="25" t="s">
         <v>37</v>
       </c>
       <c r="D4" s="3"/>
@@ -1577,10 +1592,10 @@
       <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="26" t="s">
         <v>37</v>
       </c>
       <c r="D5" s="3"/>
@@ -1605,11 +1620,15 @@
       <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="E7" t="s">
         <v>9</v>
       </c>
@@ -1644,10 +1663,10 @@
       <c r="A10" s="15">
         <v>7</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="26" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="3"/>
@@ -1663,7 +1682,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="64"/>
       <c r="E11" t="s">
         <v>36</v>
       </c>
@@ -1765,7 +1784,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27FC714-F48D-43C0-A1A9-3A577A6148C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1782,24 +1801,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="E1" s="23" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="E1" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="54"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -1822,16 +1841,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="E4" s="29" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="E4" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="31"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
@@ -1894,11 +1913,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="34"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -1932,16 +1951,16 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="E12" s="32" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="E12" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -1972,11 +1991,11 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="60"/>
       <c r="E15" s="15">
         <v>3</v>
       </c>
@@ -2076,7 +2095,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAA3160-82E3-45BC-B310-F18EC04D4CC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2091,16 +2110,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -2246,7 +2265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BEBD45-0793-4925-A547-A1D629B06294}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2261,16 +2280,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="54"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">

</xml_diff>

<commit_message>
Creados los triggers de update.
Creados los scripts de update, actualizada la lista de pendientes.
</commit_message>
<xml_diff>
--- a/LISTA DE PENDIENTES.xlsx
+++ b/LISTA DE PENDIENTES.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="TABLAS" sheetId="6" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>Alvaro</t>
-  </si>
-  <si>
-    <t>faltan los de update, inserts ya hechos</t>
   </si>
 </sst>
 </file>
@@ -710,6 +707,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,7 +774,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1080,45 +1077,45 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="52"/>
       <c r="E3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="40" t="s">
         <v>77</v>
       </c>
@@ -1537,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,22 +1543,22 @@
     <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="5" max="5" width="48.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
       <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
       <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1626,9 +1623,7 @@
       <c r="C7" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="D7" s="3"/>
       <c r="E7" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1677,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="64"/>
+      <c r="D11" s="42"/>
       <c r="E11" t="s">
         <v>36</v>
       </c>
@@ -1801,24 +1796,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
-      <c r="E1" s="52" t="s">
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
+      <c r="E1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="55"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="57"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -1841,16 +1836,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="E4" s="61" t="s">
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="E4" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="62"/>
-      <c r="G4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="64"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
@@ -1913,11 +1908,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -1951,16 +1946,16 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="59"/>
-      <c r="C12" s="60"/>
-      <c r="E12" s="58" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="E12" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -1991,11 +1986,11 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="61"/>
       <c r="E15" s="15">
         <v>3</v>
       </c>
@@ -2110,16 +2105,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -2280,16 +2275,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="55"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">

</xml_diff>

<commit_message>
Agregados procedures de insert.
</commit_message>
<xml_diff>
--- a/LISTA DE PENDIENTES.xlsx
+++ b/LISTA DE PENDIENTES.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{16CEE4E5-EFD0-43DD-AE4C-6A6DC29156B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TABLAS" sheetId="6" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
   <si>
     <t>ID</t>
   </si>
@@ -350,13 +349,13 @@
     <t>REQUISITO</t>
   </si>
   <si>
-    <t>ALVARO</t>
+    <t>Alvaro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -709,6 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,7 +775,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,7 +1054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C6C1628-72ED-4D56-9DEB-53E6C60D570F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -1079,45 +1078,45 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1"/>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="45"/>
       <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="47"/>
       <c r="J2" s="17"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="53"/>
       <c r="E3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50"/>
       <c r="I3" s="40" t="s">
         <v>76</v>
       </c>
@@ -1549,11 +1548,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1565,17 +1564,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
       <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1628,7 +1627,7 @@
         <v>37</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="43" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1643,7 +1642,7 @@
         <v>108</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="43" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1656,7 +1655,7 @@
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="43" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1695,7 +1694,9 @@
       <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
         <v>36</v>
@@ -1708,7 +1709,9 @@
       <c r="B12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="D12" s="3"/>
       <c r="E12" t="s">
         <v>50</v>
@@ -1798,7 +1801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27FC714-F48D-43C0-A1A9-3A577A6148C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1815,24 +1818,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="E1" s="53" t="s">
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="E1" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -1855,16 +1858,16 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
-      <c r="E4" s="62" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="E4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="65"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
@@ -1927,11 +1930,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
       <c r="E9" s="2">
         <v>5</v>
       </c>
@@ -1965,16 +1968,16 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="61"/>
-      <c r="E12" s="59" t="s">
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
+      <c r="E12" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="62"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
@@ -2005,11 +2008,11 @@
       <c r="G14" s="9"/>
     </row>
     <row r="15" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
       <c r="E15" s="15">
         <v>3</v>
       </c>
@@ -2109,7 +2112,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAA3160-82E3-45BC-B310-F18EC04D4CC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2124,16 +2127,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -2279,7 +2282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BEBD45-0793-4925-A547-A1D629B06294}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2294,16 +2297,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">

</xml_diff>